<commit_message>
Updated sorting and styling
</commit_message>
<xml_diff>
--- a/pocketlinux.xlsx
+++ b/pocketlinux.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" state="visible" r:id="rId2"/>
@@ -230,6 +230,12 @@
     <t xml:space="preserve">Eee Pad Transformer Prime</t>
   </si>
   <si>
+    <t xml:space="preserve">Eee Pad Transformer TF300T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See Also https://wiki.ubuntu.com/Touch/Devices/tf300t</t>
+  </si>
+  <si>
     <t xml:space="preserve">MeMO Pad 7 (ME176C(X))</t>
   </si>
   <si>
@@ -245,6 +251,9 @@
     <t xml:space="preserve">Transformer Pad 3G</t>
   </si>
   <si>
+    <t xml:space="preserve">Zenfone 2 (Z00L)</t>
+  </si>
+  <si>
     <t xml:space="preserve">ZenFone 2 Laser (720p)</t>
   </si>
   <si>
@@ -260,27 +269,18 @@
     <t xml:space="preserve">Zenfone Max</t>
   </si>
   <si>
+    <t xml:space="preserve">Zenfone Max Pro M1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zenfone Max Pro M2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Zenpad 8.0 (Z380KL)</t>
   </si>
   <si>
     <t xml:space="preserve">Zenwatch 2</t>
   </si>
   <si>
-    <t xml:space="preserve">Zenfone Max Pro M1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zenfone Max Pro M2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Also: https://wiki.ubuntu.com/Touch/Devices/tf300t</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eee Pad Transformer TF300T</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zenfone 2 (Z00L)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bliss</t>
   </si>
   <si>
@@ -302,16 +302,16 @@
     <t xml:space="preserve">Aquaris M10 HD</t>
   </si>
   <si>
+    <t xml:space="preserve">Aquaris M5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aquaris U</t>
+  </si>
+  <si>
     <t xml:space="preserve">Aquaris U Plus</t>
   </si>
   <si>
     <t xml:space="preserve">Aquaris X5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aquaris M5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aquaris U</t>
   </si>
   <si>
     <t xml:space="preserve">Aquaris X5 Plus</t>
@@ -579,8 +579,8 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right/>
+      <left/>
+      <right style="thin"/>
       <top style="thin">
         <color rgb="FF666666"/>
       </top>
@@ -590,8 +590,8 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin"/>
+      <left style="thin"/>
+      <right/>
       <top style="thin">
         <color rgb="FF666666"/>
       </top>
@@ -640,7 +640,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="48">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -789,11 +789,23 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -801,23 +813,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -835,10 +831,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -850,6 +842,51 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00A933"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9E0404"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0023FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF69EFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -918,12 +955,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:XFD1048576"/>
+  <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="3" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="3" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E56" activeCellId="0" sqref="E56"/>
+      <selection pane="bottomLeft" activeCell="I53" activeCellId="0" sqref="I53:R53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.34375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1634,6 +1671,7 @@
       <c r="H49" s="26"/>
     </row>
     <row r="50" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="3"/>
       <c r="B50" s="21" t="s">
         <v>67</v>
       </c>
@@ -1647,6 +1685,7 @@
       <c r="H50" s="26"/>
     </row>
     <row r="51" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="3"/>
       <c r="B51" s="21" t="s">
         <v>68</v>
       </c>
@@ -1660,21 +1699,25 @@
       <c r="H51" s="26"/>
     </row>
     <row r="52" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B52" s="37" t="s">
+      <c r="A52" s="3"/>
+      <c r="B52" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C52" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D52" s="24"/>
-      <c r="E52" s="24"/>
-      <c r="F52" s="24"/>
-      <c r="G52" s="24"/>
-      <c r="H52" s="38"/>
+      <c r="C52" s="37"/>
+      <c r="D52" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="37"/>
+      <c r="F52" s="37"/>
+      <c r="G52" s="37"/>
+      <c r="H52" s="39" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B53" s="37" t="s">
-        <v>70</v>
+      <c r="A53" s="3"/>
+      <c r="B53" s="40" t="s">
+        <v>71</v>
       </c>
       <c r="C53" s="22" t="s">
         <v>11</v>
@@ -1683,193 +1726,202 @@
       <c r="E53" s="24"/>
       <c r="F53" s="24"/>
       <c r="G53" s="24"/>
-      <c r="H53" s="38"/>
+      <c r="H53" s="39"/>
     </row>
     <row r="54" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B54" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C54" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="D54" s="40"/>
-      <c r="E54" s="40"/>
-      <c r="F54" s="40"/>
-      <c r="G54" s="40"/>
+      <c r="A54" s="3"/>
+      <c r="B54" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="C54" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54" s="24"/>
+      <c r="E54" s="24"/>
+      <c r="F54" s="24"/>
+      <c r="G54" s="24"/>
       <c r="H54" s="41"/>
     </row>
     <row r="55" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="3"/>
       <c r="B55" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C55" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="D55" s="40"/>
-      <c r="E55" s="40"/>
-      <c r="F55" s="40"/>
-      <c r="G55" s="40"/>
+        <v>73</v>
+      </c>
+      <c r="C55" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" s="37"/>
+      <c r="E55" s="37"/>
+      <c r="F55" s="37"/>
+      <c r="G55" s="37"/>
       <c r="H55" s="41"/>
     </row>
     <row r="56" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="3"/>
       <c r="B56" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C56" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="D56" s="40"/>
-      <c r="E56" s="40"/>
-      <c r="F56" s="40"/>
-      <c r="G56" s="40"/>
+        <v>74</v>
+      </c>
+      <c r="C56" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56" s="37"/>
+      <c r="E56" s="37"/>
+      <c r="F56" s="37"/>
+      <c r="G56" s="37"/>
       <c r="H56" s="41"/>
     </row>
     <row r="57" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="3"/>
       <c r="B57" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C57" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="D57" s="40"/>
-      <c r="E57" s="40"/>
-      <c r="F57" s="40"/>
-      <c r="G57" s="40"/>
+        <v>75</v>
+      </c>
+      <c r="C57" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D57" s="37"/>
+      <c r="E57" s="37"/>
+      <c r="F57" s="37"/>
+      <c r="G57" s="37"/>
       <c r="H57" s="41"/>
     </row>
     <row r="58" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="3"/>
       <c r="B58" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C58" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="D58" s="40"/>
-      <c r="E58" s="40"/>
-      <c r="F58" s="40"/>
-      <c r="G58" s="40"/>
+        <v>76</v>
+      </c>
+      <c r="C58" s="37"/>
+      <c r="D58" s="37"/>
+      <c r="E58" s="37"/>
+      <c r="F58" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G58" s="37"/>
       <c r="H58" s="41"/>
     </row>
     <row r="59" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="3"/>
       <c r="B59" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C59" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="D59" s="40"/>
-      <c r="E59" s="40"/>
-      <c r="F59" s="40"/>
-      <c r="G59" s="40"/>
+        <v>77</v>
+      </c>
+      <c r="C59" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D59" s="37"/>
+      <c r="E59" s="37"/>
+      <c r="F59" s="37"/>
+      <c r="G59" s="37"/>
       <c r="H59" s="41"/>
     </row>
     <row r="60" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="3"/>
       <c r="B60" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C60" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="D60" s="40"/>
-      <c r="E60" s="40"/>
-      <c r="F60" s="40"/>
-      <c r="G60" s="40"/>
+        <v>78</v>
+      </c>
+      <c r="C60" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D60" s="37"/>
+      <c r="E60" s="37"/>
+      <c r="F60" s="37"/>
+      <c r="G60" s="37"/>
       <c r="H60" s="41"/>
     </row>
     <row r="61" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="3"/>
       <c r="B61" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C61" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="D61" s="40"/>
-      <c r="E61" s="40"/>
-      <c r="F61" s="40"/>
-      <c r="G61" s="40"/>
+        <v>79</v>
+      </c>
+      <c r="C61" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D61" s="37"/>
+      <c r="E61" s="37"/>
+      <c r="F61" s="37"/>
+      <c r="G61" s="37"/>
       <c r="H61" s="41"/>
     </row>
     <row r="62" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="3"/>
       <c r="B62" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C62" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="D62" s="40"/>
-      <c r="E62" s="40"/>
-      <c r="F62" s="40"/>
-      <c r="G62" s="40"/>
+        <v>80</v>
+      </c>
+      <c r="C62" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D62" s="37"/>
+      <c r="E62" s="37"/>
+      <c r="F62" s="37"/>
+      <c r="G62" s="37"/>
       <c r="H62" s="41"/>
     </row>
     <row r="63" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="3"/>
       <c r="B63" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C63" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="D63" s="40"/>
-      <c r="E63" s="40"/>
-      <c r="F63" s="40"/>
-      <c r="G63" s="40"/>
+        <v>81</v>
+      </c>
+      <c r="C63" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D63" s="37"/>
+      <c r="E63" s="37"/>
+      <c r="F63" s="37"/>
+      <c r="G63" s="37"/>
       <c r="H63" s="41"/>
     </row>
     <row r="64" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B64" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C64" s="18"/>
-      <c r="D64" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="E64" s="18"/>
-      <c r="F64" s="18"/>
-      <c r="G64" s="18"/>
-      <c r="H64" s="18"/>
+      <c r="A64" s="3"/>
+      <c r="B64" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C64" s="37"/>
+      <c r="D64" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E64" s="37"/>
+      <c r="F64" s="37"/>
+      <c r="G64" s="37"/>
+      <c r="H64" s="41"/>
     </row>
     <row r="65" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B65" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C65" s="18"/>
-      <c r="D65" s="18"/>
+      <c r="A65" s="3"/>
+      <c r="B65" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C65" s="37"/>
+      <c r="D65" s="37"/>
       <c r="E65" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="F65" s="18"/>
-      <c r="G65" s="18"/>
-      <c r="H65" s="18"/>
+      <c r="F65" s="37"/>
+      <c r="G65" s="37"/>
+      <c r="H65" s="41"/>
     </row>
     <row r="66" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B66" s="3" t="s">
+      <c r="B66" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C66" s="18"/>
-      <c r="D66" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="E66" s="18"/>
-      <c r="F66" s="18"/>
-      <c r="G66" s="18"/>
-      <c r="H66" s="18"/>
-      <c r="XFD66" s="0"/>
+      <c r="C66" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D66" s="37"/>
+      <c r="E66" s="37"/>
+      <c r="F66" s="37"/>
+      <c r="G66" s="37"/>
+      <c r="H66" s="41"/>
     </row>
     <row r="67" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B67" s="3" t="s">
+      <c r="A67" s="44"/>
+      <c r="B67" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C67" s="18"/>
-      <c r="D67" s="18"/>
-      <c r="E67" s="18"/>
-      <c r="F67" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="G67" s="18"/>
-      <c r="H67" s="18"/>
+      <c r="C67" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D67" s="37"/>
+      <c r="E67" s="37"/>
+      <c r="F67" s="37"/>
+      <c r="G67" s="37"/>
+      <c r="H67" s="41"/>
     </row>
     <row r="68" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B68" s="3"/>
@@ -2025,32 +2077,33 @@
       <c r="H84" s="18"/>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B88" s="45"/>
-      <c r="C88" s="45"/>
-      <c r="D88" s="45"/>
-      <c r="E88" s="45"/>
-      <c r="F88" s="45"/>
-      <c r="G88" s="45"/>
-      <c r="H88" s="45"/>
+      <c r="B88" s="44"/>
+      <c r="C88" s="44"/>
+      <c r="D88" s="44"/>
+      <c r="E88" s="44"/>
+      <c r="F88" s="44"/>
+      <c r="G88" s="44"/>
+      <c r="H88" s="44"/>
     </row>
     <row r="91" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B104" s="45"/>
-      <c r="C104" s="45"/>
-      <c r="D104" s="45"/>
-      <c r="E104" s="45"/>
-      <c r="F104" s="45"/>
-      <c r="G104" s="45"/>
-      <c r="H104" s="45"/>
+      <c r="B104" s="44"/>
+      <c r="C104" s="44"/>
+      <c r="D104" s="44"/>
+      <c r="E104" s="44"/>
+      <c r="F104" s="44"/>
+      <c r="G104" s="44"/>
+      <c r="H104" s="44"/>
     </row>
     <row r="107" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:C2"/>
     <mergeCell ref="A4:A13"/>
     <mergeCell ref="A14:A27"/>
+    <mergeCell ref="A50:A65"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" display="yes"/>
@@ -2095,23 +2148,23 @@
     <hyperlink ref="C49" r:id="rId40" display="yes"/>
     <hyperlink ref="C50" r:id="rId41" display="yes"/>
     <hyperlink ref="C51" r:id="rId42" display="yes"/>
-    <hyperlink ref="C52" r:id="rId43" display="yes"/>
-    <hyperlink ref="C53" r:id="rId44" display="yes"/>
-    <hyperlink ref="C54" r:id="rId45" display="yes"/>
-    <hyperlink ref="C55" r:id="rId46" display="yes"/>
-    <hyperlink ref="C56" r:id="rId47" display="yes"/>
-    <hyperlink ref="C57" r:id="rId48" display="yes"/>
-    <hyperlink ref="C58" r:id="rId49" display="yes"/>
-    <hyperlink ref="C59" r:id="rId50" display="yes"/>
-    <hyperlink ref="C60" r:id="rId51" display="yes"/>
-    <hyperlink ref="C61" r:id="rId52" display="yes"/>
-    <hyperlink ref="C62" r:id="rId53" display="yes"/>
-    <hyperlink ref="C63" r:id="rId54" display="yes"/>
-    <hyperlink ref="D64" r:id="rId55" display="yes"/>
-    <hyperlink ref="E65" r:id="rId56" display="yes"/>
-    <hyperlink ref="A66" r:id="rId57" display="https://wiki.ubuntu.com/Touch/Devices/tf300t"/>
-    <hyperlink ref="D66" r:id="rId58" display="yes"/>
-    <hyperlink ref="F67" r:id="rId59" display="yes"/>
+    <hyperlink ref="D52" r:id="rId43" display="yes"/>
+    <hyperlink ref="H52" r:id="rId44" display="https://wiki.ubuntu.com/Touch/Devices/tf300t"/>
+    <hyperlink ref="C53" r:id="rId45" display="yes"/>
+    <hyperlink ref="C54" r:id="rId46" display="yes"/>
+    <hyperlink ref="C55" r:id="rId47" display="yes"/>
+    <hyperlink ref="C56" r:id="rId48" display="yes"/>
+    <hyperlink ref="C57" r:id="rId49" display="yes"/>
+    <hyperlink ref="F58" r:id="rId50" display="yes"/>
+    <hyperlink ref="C59" r:id="rId51" display="yes"/>
+    <hyperlink ref="C60" r:id="rId52" display="yes"/>
+    <hyperlink ref="C61" r:id="rId53" display="yes"/>
+    <hyperlink ref="C62" r:id="rId54" display="yes"/>
+    <hyperlink ref="C63" r:id="rId55" display="yes"/>
+    <hyperlink ref="D64" r:id="rId56" display="yes"/>
+    <hyperlink ref="E65" r:id="rId57" display="yes"/>
+    <hyperlink ref="C66" r:id="rId58" display="yes"/>
+    <hyperlink ref="C67" r:id="rId59" display="yes"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2128,12 +2181,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:XFD107"/>
+  <dimension ref="A1:H107"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="F9" activeCellId="1" sqref="I53:R53 F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.34375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2193,125 +2246,125 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="45" t="s">
         <v>86</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="47" t="s">
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="46" t="s">
         <v>11</v>
       </c>
       <c r="H4" s="41"/>
     </row>
     <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="47" t="s">
         <v>88</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="49" t="s">
+      <c r="C5" s="37"/>
+      <c r="D5" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
       <c r="H5" s="41"/>
     </row>
     <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="48"/>
+      <c r="A6" s="47"/>
       <c r="B6" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C6" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="49" t="s">
+      <c r="C6" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
       <c r="H6" s="41"/>
     </row>
     <row r="7" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="48"/>
+      <c r="A7" s="47"/>
       <c r="B7" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="49" t="s">
+      <c r="C7" s="37"/>
+      <c r="D7" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
       <c r="H7" s="41"/>
     </row>
     <row r="8" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="48"/>
+      <c r="A8" s="47"/>
       <c r="B8" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="49" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
+      <c r="C8" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
       <c r="H8" s="41"/>
     </row>
     <row r="9" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="48"/>
-      <c r="B9" s="5" t="s">
+      <c r="A9" s="47"/>
+      <c r="B9" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C9" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
+      <c r="C9" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
       <c r="H9" s="41"/>
     </row>
     <row r="10" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="48"/>
+      <c r="A10" s="47"/>
       <c r="B10" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C10" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
       <c r="H10" s="41"/>
     </row>
     <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="48"/>
-      <c r="B11" s="4" t="s">
+      <c r="A11" s="47"/>
+      <c r="B11" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C11" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
+      <c r="C11" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
       <c r="H11" s="41"/>
     </row>
     <row r="12" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="48"/>
+      <c r="A12" s="47"/>
       <c r="B12" s="13" t="s">
         <v>97</v>
       </c>
@@ -2400,13 +2453,13 @@
     <row r="22" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="45"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="45"/>
-      <c r="G24" s="45"/>
-      <c r="H24" s="45"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="44"/>
     </row>
     <row r="25" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="26" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2424,13 +2477,13 @@
     <row r="38" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="39" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="40" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B40" s="45"/>
-      <c r="C40" s="45"/>
-      <c r="D40" s="45"/>
-      <c r="E40" s="45"/>
-      <c r="F40" s="45"/>
-      <c r="G40" s="45"/>
-      <c r="H40" s="45"/>
+      <c r="B40" s="44"/>
+      <c r="C40" s="44"/>
+      <c r="D40" s="44"/>
+      <c r="E40" s="44"/>
+      <c r="F40" s="44"/>
+      <c r="G40" s="44"/>
+      <c r="H40" s="44"/>
     </row>
     <row r="41" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="42" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2457,9 +2510,7 @@
     <row r="63" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="64" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="65" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="66" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="XFD66" s="0"/>
-    </row>
+    <row r="66" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="67" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="68" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="69" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2487,13 +2538,13 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G4" r:id="rId1" display="yes"/>
-    <hyperlink ref="D5" r:id="rId2" display="yes"/>
+    <hyperlink ref="D5" r:id="rId2" display="yes(native)"/>
     <hyperlink ref="C6" r:id="rId3" display="yes"/>
-    <hyperlink ref="D6" r:id="rId4" display="yes"/>
-    <hyperlink ref="D7" r:id="rId5" display="yes"/>
-    <hyperlink ref="D8" r:id="rId6" display="yes"/>
+    <hyperlink ref="D6" r:id="rId4" display="yes(native)"/>
+    <hyperlink ref="D7" r:id="rId5" display="yes(native)"/>
+    <hyperlink ref="C8" r:id="rId6" display="yes"/>
     <hyperlink ref="C9" r:id="rId7" display="yes"/>
-    <hyperlink ref="C10" r:id="rId8" display="yes"/>
+    <hyperlink ref="D10" r:id="rId8" display="yes"/>
     <hyperlink ref="C11" r:id="rId9" display="yes"/>
     <hyperlink ref="C12" r:id="rId10" display="yes"/>
   </hyperlinks>

</xml_diff>